<commit_message>
added the measurements from Feb 5 into ROV sheet. Mean calculation, isolating 1 site, dont know how to put them all together again though
</commit_message>
<xml_diff>
--- a/historic_raw_data/ISA_data_all.xlsx
+++ b/historic_raw_data/ISA_data_all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicole/Desktop/honours_project/raw data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicole/Desktop/honours_project/pink_sea_star_indian_arm/historic_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F0A17B-72A6-E64E-B7F1-E9C2EBEC857E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9305679-FB16-7F45-9ACF-96F370A01E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{D93A6C75-FF0D-4F4B-BD74-1F16D807F5AB}"/>
+    <workbookView xWindow="32740" yWindow="-10300" windowWidth="46380" windowHeight="24180" xr2:uid="{D93A6C75-FF0D-4F4B-BD74-1F16D807F5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,8 +621,8 @@
   <dimension ref="A1:M393"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H306" sqref="H306"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11812,6 +11812,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>